<commit_message>
Exercicio 3 - Normalizacao, criacao de db, tabelas e relacoes - Step 3
</commit_message>
<xml_diff>
--- a/3-back-end/bloco-21-funcoes-sql-joins-e-normalizacao/dia-3-transformando-ideias-em-um-modelo-de-banco-de-dados/Exercicios de normalizacao de dados.xlsx
+++ b/3-back-end/bloco-21-funcoes-sql-joins-e-normalizacao/dia-3-transformando-ideias-em-um-modelo-de-banco-de-dados/Exercicios de normalizacao de dados.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
   <si>
     <t xml:space="preserve">Exercício 1: 🚀 Normalize a tabela a seguir para a 1ª Forma Normal.</t>
   </si>
@@ -576,14 +576,14 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1715400</xdr:colOff>
+      <xdr:colOff>1715760</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>153000</xdr:rowOff>
+      <xdr:rowOff>153360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>520200</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>9360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -597,8 +597,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5661720" y="6532560"/>
-          <a:ext cx="6372000" cy="2327760"/>
+          <a:off x="5664600" y="6532920"/>
+          <a:ext cx="6371640" cy="2685600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -618,13 +618,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:I56"/>
+  <dimension ref="B2:I57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D48" activeCellId="0" sqref="D48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.52"/>
@@ -1125,70 +1125,123 @@
       <c r="C41" s="3"/>
       <c r="I41" s="11"/>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="9"/>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" s="2"/>
       <c r="I42" s="11"/>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="9"/>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="14" t="n">
+        <v>12</v>
+      </c>
+      <c r="C43" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D43" s="20"/>
       <c r="I43" s="11"/>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="9"/>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="14" t="n">
+        <v>12</v>
+      </c>
+      <c r="C44" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="D44" s="20"/>
       <c r="I44" s="11"/>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="9"/>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="14" t="n">
+        <v>13</v>
+      </c>
+      <c r="C45" s="20" t="n">
+        <v>2</v>
+      </c>
+      <c r="D45" s="20"/>
       <c r="I45" s="11"/>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="9"/>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="14" t="n">
+        <v>14</v>
+      </c>
+      <c r="C46" s="20" t="n">
+        <v>3</v>
+      </c>
+      <c r="D46" s="20"/>
       <c r="I46" s="11"/>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="9"/>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="14" t="n">
+        <v>14</v>
+      </c>
+      <c r="C47" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="D47" s="20"/>
       <c r="I47" s="11"/>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="17"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18"/>
-      <c r="I48" s="19"/>
-    </row>
-    <row r="50" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="1" t="s">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="14" t="n">
+        <v>15</v>
+      </c>
+      <c r="C48" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="D48" s="20"/>
+      <c r="I48" s="11"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="17"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="19"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="1" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C51" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C54" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="12">
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>